<commit_message>
cleaned script and added comments
added lineitem comments and test files
</commit_message>
<xml_diff>
--- a/tests/Project Workflow Export (Sample Data).xlsx
+++ b/tests/Project Workflow Export (Sample Data).xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workflow-comment-parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workflow-comment-parser\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF0936E-09B7-42A6-8C04-755A86BFB878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3679B3-442B-45E5-81C8-695DB8289BF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="6" r:id="rId1"/>
@@ -589,18 +589,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I5" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I5" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Plan Name" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task Title" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Bucket" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Assigned to" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start date" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Due date" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Completed by" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Completed date" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Plan Name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task Title" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Bucket" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Assigned to" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start date" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Due date" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Completed by" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Completed date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -905,18 +905,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="117.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" style="1" customWidth="1"/>
     <col min="5" max="6" width="16.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="215.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="70" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
@@ -994,7 +994,7 @@
         <v>44159.083333333299</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>